<commit_message>
Updated sprint velocity for Sprint 2
</commit_message>
<xml_diff>
--- a/docs/sprint/Sprint Velocity.xlsx
+++ b/docs/sprint/Sprint Velocity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="11235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25607" windowHeight="11233"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,20 +350,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.41015625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,7 +374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -385,12 +385,23 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>26</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sprint velocity for sprint 4
</commit_message>
<xml_diff>
--- a/docs/sprint/Sprint Velocity.xlsx
+++ b/docs/sprint/Sprint Velocity.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -403,6 +403,17 @@
       <c r="B4">
         <v>34</v>
       </c>
+      <c r="C4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update sprint 4 velocity spreadsheet
</commit_message>
<xml_diff>
--- a/docs/sprint/Sprint Velocity.xlsx
+++ b/docs/sprint/Sprint Velocity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25607" windowHeight="11233"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,20 +350,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,7 +374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -385,7 +385,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -396,7 +396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -407,12 +407,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>25</v>
+      </c>
+      <c r="C5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>